<commit_message>
edited the system test report
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_87EC0788E23DDDB5A58E58ABB6DADC2DBD3A7C1E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D750591-AD94-445D-BC3D-048EC555FF67}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Test Report" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases &amp; Results" sheetId="1" r:id="rId2"/>
     <sheet name="Enums" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -20,6 +21,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="80">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -41,12 +44,6 @@
     <t>Not Tested</t>
   </si>
   <si>
-    <t>TestCase_ID</t>
-  </si>
-  <si>
-    <t>Requirement_ID</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Expected Result</t>
   </si>
   <si>
-    <t>Actual Result</t>
-  </si>
-  <si>
     <t>Test Result</t>
   </si>
   <si>
@@ -83,25 +77,221 @@
     <t>Low Impact</t>
   </si>
   <si>
-    <t>Test that the water heater is activated if the water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
-    <t>Water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
-    <t>From the LCD main menu, select the option "Black Coffee"</t>
-  </si>
-  <si>
-    <t>-Heating element is activated when water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
-    <t>REQ-06</t>
+    <t>1. Simulate temp rising to 45°C.</t>
+  </si>
+  <si>
+    <t>Actual result</t>
+  </si>
+  <si>
+    <t>2. Observe system logs/alerts.</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Verify temp &amp; humidity sensor triggers fire alert at &gt;40°C</t>
+  </si>
+  <si>
+    <t>System powered on, sensor connected</t>
+  </si>
+  <si>
+    <t>1. Simulate temp rising to 45°C
+2. Monitor readings
+3. Check alert status</t>
+  </si>
+  <si>
+    <t>Fire alert triggered</t>
+  </si>
+  <si>
+    <t>Flame detected, false alarm rejected</t>
+  </si>
+  <si>
+    <t>Verify IR sensor detects flames via flickering IR patterns</t>
+  </si>
+  <si>
+    <t>Mock heat source available, sensor connected</t>
+  </si>
+  <si>
+    <t>1. Place controlled flame near IR sensor
+2. Place hot object (non-flame) for false alarm test</t>
+  </si>
+  <si>
+    <t>LDR value decreases, smoke alert triggered</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Verify LDR detects smoke</t>
+  </si>
+  <si>
+    <t>mock room lit, system on</t>
+  </si>
+  <si>
+    <t>1. Introduce smoke (incense stick)
+2. Observe LDR readings</t>
+  </si>
+  <si>
+    <t>Camera feed visible on system</t>
+  </si>
+  <si>
+    <t>Verify ultrasonic sensor detects human presence</t>
+  </si>
+  <si>
+    <t>mock room empty, system running</t>
+  </si>
+  <si>
+    <t>1. Walk in front of sensor
+2. Observe detection status</t>
+  </si>
+  <si>
+    <t>Human presence correctly detected</t>
+  </si>
+  <si>
+    <t>Moisture detected if water is released</t>
+  </si>
+  <si>
+    <t>Verify moisture sensor detects sprinkler activation</t>
+  </si>
+  <si>
+    <t>Mock Sprinkler functional</t>
+  </si>
+  <si>
+    <t>1. Activate sprinkler
+2. Check moisture sensor output</t>
+  </si>
+  <si>
+    <t>Alert triggered immediately</t>
+  </si>
+  <si>
+    <t>Verify system triggers fire alert on any sensor input</t>
+  </si>
+  <si>
+    <t>Mock System on</t>
+  </si>
+  <si>
+    <t>1. Trigger sensor (temp &gt;40°C or IR flame)
+2. Observe system</t>
+  </si>
+  <si>
+    <t>Camera input enhances confirmation</t>
+  </si>
+  <si>
+    <t>Verify ultrasonic sensor detects presence during fire</t>
+  </si>
+  <si>
+    <t>Mock Person inside room</t>
+  </si>
+  <si>
+    <t>1. Trigger fire event
+2. Check if occupant presence is detected</t>
+  </si>
+  <si>
+    <t>Occupant detection logged</t>
+  </si>
+  <si>
+    <t>Notification sent to SCDF + residents</t>
+  </si>
+  <si>
+    <t>Verify system notifies SCDF &amp; residents</t>
+  </si>
+  <si>
+    <t>Mock Fire detected</t>
+  </si>
+  <si>
+    <t>1. Simulate fire
+2. Check telegram/email logs</t>
+  </si>
+  <si>
+    <t>System armed after card detected</t>
+  </si>
+  <si>
+    <t>Verify system activates only after RFID card detected</t>
+  </si>
+  <si>
+    <t>Mock RFID card registered</t>
+  </si>
+  <si>
+    <t>1. Scan valid RFID card
+2. Observe system</t>
+  </si>
+  <si>
+    <t>Wrong code rejected, correct code stops alarm</t>
+  </si>
+  <si>
+    <t>Verify keypad can deactivate alert with correct code</t>
+  </si>
+  <si>
+    <t>Mock System in alarm state</t>
+  </si>
+  <si>
+    <t>1. Enter wrong code
+2. Enter correct code</t>
+  </si>
+  <si>
+    <t>Servo opens valve, water released</t>
+  </si>
+  <si>
+    <t>Verify sprinkler activates via servo motor</t>
+  </si>
+  <si>
+    <t>1. Trigger fire event
+2. Observe servo motor action</t>
+  </si>
+  <si>
+    <t>Window opens automatically</t>
+  </si>
+  <si>
+    <t>Verify DC motor opens window during fire</t>
+  </si>
+  <si>
+    <t>Mock Fire detected, motor installed</t>
+  </si>
+  <si>
+    <t>1. Trigger fire event
+2. Observe motor action</t>
+  </si>
+  <si>
+    <t>System detects failure (no water)</t>
+  </si>
+  <si>
+    <t>Verify LCD screen shows fire alert</t>
+  </si>
+  <si>
+    <t>Mock Fire simulated</t>
+  </si>
+  <si>
+    <t>1. Trigger fire
+2. Observe LCD</t>
+  </si>
+  <si>
+    <t>Alert message shown</t>
+  </si>
+  <si>
+    <t>Loud alarm activated</t>
+  </si>
+  <si>
+    <t>Verify buzzer alarm activates</t>
+  </si>
+  <si>
+    <t>1. Trigger fire
+2. Observe buzzer</t>
+  </si>
+  <si>
+    <t>Residents + SCDF notified</t>
+  </si>
+  <si>
+    <t>Verify notifications sent via telegram/email</t>
+  </si>
+  <si>
+    <t>1. Trigger fire
+2. Check alerts on devices</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,18 +382,8 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -222,21 +402,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -248,13 +433,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -311,7 +489,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -487,13 +664,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1208,9 +1385,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1248,9 +1425,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1285,7 +1462,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1320,7 +1497,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1493,52 +1670,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView zoomScale="129" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="6">
         <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="6">
         <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Pass")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="6">
         <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Fail")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="6">
         <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1549,433 +1726,663 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="51" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="28.1796875" customWidth="1"/>
+    <col min="7" max="7" width="21.7265625" customWidth="1"/>
+    <col min="8" max="8" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" customWidth="1"/>
+    <col min="11" max="11" width="12.54296875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="12"/>
+      <c r="B3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="12"/>
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="12"/>
+      <c r="B5" s="11">
+        <v>2</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="12"/>
+      <c r="B6" s="11">
+        <v>3</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="12"/>
+      <c r="B7" s="11">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="12"/>
+      <c r="B8" s="11">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="C8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="12"/>
+      <c r="B9" s="11">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="C9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="12"/>
+      <c r="B10" s="11">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="C10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="12"/>
+      <c r="B11" s="11">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="C11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="12"/>
+      <c r="B12" s="11">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="C12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="12"/>
+      <c r="B13" s="11">
         <v>10</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="11" t="s">
+      <c r="C13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="12"/>
+      <c r="B14" s="11">
+        <v>11</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="12"/>
+      <c r="B15" s="11">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+      <c r="C15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
+      <c r="B16" s="11">
+        <v>13</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="12"/>
+      <c r="B17" s="11">
+        <v>14</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="12"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B20" s="1">
+        <f t="shared" ref="B5:B20" si="0">B19+1</f>
         <v>1</v>
       </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <f>B3+1</f>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B21" s="1">
+        <f t="shared" ref="B21:B22" si="1">B20+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="12" t="s">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <f t="shared" ref="B5:B20" si="0">B4+1</f>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B22" s="1">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="12" t="s">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
-        <f t="shared" ref="B21:B22" si="1">B20+1</f>
-        <v>19</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+  <conditionalFormatting sqref="K3:K22">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1983,13 +2390,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Enums!$B$8:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>E3:E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -2002,43 +2409,43 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2048,21 +2455,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E81D8C8DDAE8BD44A422697963F06C45" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6816e004dbb89c674e51f5647972552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b02348f-b4e3-458c-83fc-9e90db0f8029" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6418ca14ac9ee17b8bbf6df78e0c223" ns2:_="">
     <xsd:import namespace="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
@@ -2220,31 +2612,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2260,4 +2643,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>